<commit_message>
Generate Groups in excel file
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">ИНФОРМАЦИЯ О НАПРАВЛЕНИЯХ</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t xml:space="preserve">ИНФОРМАЦИЯ О ГРУППАХ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СВОБОДНЫХ МЕСТ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МУЖЧИН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЖЕНЩИН</t>
   </si>
 </sst>
 </file>
@@ -130,10 +139,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -141,6 +150,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -153,6 +165,15 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>